<commit_message>
fix bus in Config
</commit_message>
<xml_diff>
--- a/Assets/Excel/CardPile.xlsx
+++ b/Assets/Excel/CardPile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityWorkSpace\NewStart\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB3296C-1E3D-4E1D-8451-4F274E975988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BD7B9E-5A93-4AEF-BDD6-209AED2965A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14664" yWindow="948" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5628" yWindow="1104" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="牌堆#CardPile#" sheetId="1" r:id="rId1"/>
@@ -646,7 +646,7 @@
   <dimension ref="A1:D164"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="D164" sqref="D164"/>
+      <selection activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update ui when switch cur player
</commit_message>
<xml_diff>
--- a/Assets/Excel/CardPile.xlsx
+++ b/Assets/Excel/CardPile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UnityWorkSpace\NewStart\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BD7B9E-5A93-4AEF-BDD6-209AED2965A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BADA25-D36E-4498-A40B-F78AAFB96570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5628" yWindow="1104" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,294 +25,288 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="69">
   <si>
     <t>int</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Suit</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Rank</t>
   </si>
   <si>
     <t>Id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>string</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>杀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>雷杀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>闪</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>桃</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>酒</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>桃园结义</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>万箭齐发</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>借刀杀人</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>五谷丰登</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>南蛮入侵</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>决斗</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>火攻</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>无中生有</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>顺手牵羊</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>过河拆桥</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>铁索连环</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>无懈可击</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>闪电</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>兵粮寸断</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>乐不思蜀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>诸葛连弩</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>青釭剑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>寒冰箭</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>雌雄双股剑</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>古锭刀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>青龙偃月刀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>丈八蛇矛</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>贯石斧</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>朱雀羽扇</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>方天画戟</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>麒麟弓</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>白银狮子</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>仁王盾</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>藤甲</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>八卦阵</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>紫骍</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>赤兔</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>大宛</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>骅骝</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>的卢</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>爪黄飞电</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>绝影</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>木牛流马</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>火杀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>♦️</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>♥️</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>♣️</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>♠️</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jiu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>taoyuan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wanjian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jiedao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wugu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nanman</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>juedou</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>huogong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wuzhong</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shunshou</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>guochai</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tiesuo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wuxie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shandian</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bingliang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,24 +315,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Segoe UI Emoji"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -361,8 +342,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -643,38 +625,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D164"/>
+  <dimension ref="A2:E164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="G158" sqref="G158"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="H139" sqref="H139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="C1" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -687,8 +669,11 @@
       <c r="D3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -701,8 +686,11 @@
       <c r="D4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -715,8 +703,11 @@
       <c r="D5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -729,8 +720,11 @@
       <c r="D6">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -743,8 +737,11 @@
       <c r="D7">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -757,8 +754,11 @@
       <c r="D8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -771,8 +771,11 @@
       <c r="D9">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -785,8 +788,11 @@
       <c r="D10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -799,8 +805,11 @@
       <c r="D11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -813,8 +822,11 @@
       <c r="D12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -827,8 +839,11 @@
       <c r="D13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -841,8 +856,11 @@
       <c r="D14">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -855,8 +873,11 @@
       <c r="D15">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -869,8 +890,11 @@
       <c r="D16">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -883,8 +907,11 @@
       <c r="D17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -897,8 +924,11 @@
       <c r="D18">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -911,8 +941,11 @@
       <c r="D19">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -925,8 +958,11 @@
       <c r="D20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -939,8 +975,11 @@
       <c r="D21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -953,8 +992,11 @@
       <c r="D22">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -967,8 +1009,11 @@
       <c r="D23">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -981,8 +1026,11 @@
       <c r="D24">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -995,8 +1043,11 @@
       <c r="D25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -1009,8 +1060,11 @@
       <c r="D26">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1023,8 +1077,11 @@
       <c r="D27">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -1037,8 +1094,11 @@
       <c r="D28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -1051,8 +1111,11 @@
       <c r="D29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -1065,8 +1128,11 @@
       <c r="D30">
         <v>9</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -1079,8 +1145,11 @@
       <c r="D31">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -1093,8 +1162,11 @@
       <c r="D32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -1107,8 +1179,11 @@
       <c r="D33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -1121,8 +1196,11 @@
       <c r="D34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -1135,8 +1213,11 @@
       <c r="D35">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -1149,8 +1230,11 @@
       <c r="D36">
         <v>7</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -1163,8 +1247,11 @@
       <c r="D37">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -1177,8 +1264,11 @@
       <c r="D38">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -1191,8 +1281,11 @@
       <c r="D39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -1205,8 +1298,11 @@
       <c r="D40">
         <v>6</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -1219,8 +1315,11 @@
       <c r="D41">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -1233,8 +1332,11 @@
       <c r="D42">
         <v>8</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -1247,8 +1349,11 @@
       <c r="D43">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
@@ -1261,8 +1366,11 @@
       <c r="D44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
@@ -1275,8 +1383,11 @@
       <c r="D45">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
@@ -1289,8 +1400,11 @@
       <c r="D46">
         <v>7</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
@@ -1303,8 +1417,11 @@
       <c r="D47">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
@@ -1317,8 +1434,11 @@
       <c r="D48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -1331,8 +1451,11 @@
       <c r="D49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -1345,8 +1468,11 @@
       <c r="D50">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
@@ -1359,8 +1485,11 @@
       <c r="D51">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
@@ -1373,8 +1502,11 @@
       <c r="D52">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -1387,8 +1519,11 @@
       <c r="D53">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -1401,8 +1536,11 @@
       <c r="D54">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
@@ -1415,8 +1553,11 @@
       <c r="D55">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -1429,8 +1570,11 @@
       <c r="D56">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -1443,8 +1587,11 @@
       <c r="D57">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -1457,8 +1604,11 @@
       <c r="D58">
         <v>8</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
@@ -1471,8 +1621,11 @@
       <c r="D59">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
@@ -1485,8 +1638,11 @@
       <c r="D60">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
@@ -1499,8 +1655,11 @@
       <c r="D61">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
@@ -1513,8 +1672,11 @@
       <c r="D62">
         <v>11</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
@@ -1527,8 +1689,11 @@
       <c r="D63">
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
@@ -1541,8 +1706,11 @@
       <c r="D64">
         <v>11</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>62</v>
       </c>
@@ -1555,8 +1723,11 @@
       <c r="D65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>63</v>
       </c>
@@ -1569,8 +1740,11 @@
       <c r="D66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>64</v>
       </c>
@@ -1583,8 +1757,11 @@
       <c r="D67">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>65</v>
       </c>
@@ -1597,8 +1774,11 @@
       <c r="D68">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>66</v>
       </c>
@@ -1611,8 +1791,11 @@
       <c r="D69">
         <v>11</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>67</v>
       </c>
@@ -1625,8 +1808,11 @@
       <c r="D70">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>68</v>
       </c>
@@ -1639,8 +1825,11 @@
       <c r="D71">
         <v>13</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>69</v>
       </c>
@@ -1653,8 +1842,11 @@
       <c r="D72">
         <v>2</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>70</v>
       </c>
@@ -1667,8 +1859,11 @@
       <c r="D73">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>71</v>
       </c>
@@ -1681,8 +1876,11 @@
       <c r="D74">
         <v>12</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
@@ -1695,8 +1893,11 @@
       <c r="D75">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>73</v>
       </c>
@@ -1709,8 +1910,11 @@
       <c r="D76">
         <v>4</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>74</v>
       </c>
@@ -1723,8 +1927,11 @@
       <c r="D77">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>75</v>
       </c>
@@ -1737,8 +1944,11 @@
       <c r="D78">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>76</v>
       </c>
@@ -1751,8 +1961,11 @@
       <c r="D79">
         <v>6</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>77</v>
       </c>
@@ -1765,8 +1978,11 @@
       <c r="D80">
         <v>7</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>78</v>
       </c>
@@ -1779,8 +1995,11 @@
       <c r="D81">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>79</v>
       </c>
@@ -1793,8 +2012,11 @@
       <c r="D82">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>80</v>
       </c>
@@ -1807,8 +2029,11 @@
       <c r="D83">
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>81</v>
       </c>
@@ -1821,8 +2046,11 @@
       <c r="D84">
         <v>9</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>82</v>
       </c>
@@ -1835,8 +2063,11 @@
       <c r="D85">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>83</v>
       </c>
@@ -1849,8 +2080,11 @@
       <c r="D86">
         <v>9</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>84</v>
       </c>
@@ -1863,8 +2097,11 @@
       <c r="D87">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>85</v>
       </c>
@@ -1877,8 +2114,11 @@
       <c r="D88">
         <v>9</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>86</v>
       </c>
@@ -1891,8 +2131,11 @@
       <c r="D89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>87</v>
       </c>
@@ -1905,8 +2148,11 @@
       <c r="D90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>88</v>
       </c>
@@ -1919,8 +2165,11 @@
       <c r="D91">
         <v>12</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>89</v>
       </c>
@@ -1933,8 +2182,11 @@
       <c r="D92">
         <v>13</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>90</v>
       </c>
@@ -1947,8 +2199,11 @@
       <c r="D93">
         <v>3</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>91</v>
       </c>
@@ -1961,8 +2216,11 @@
       <c r="D94">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>92</v>
       </c>
@@ -1975,8 +2233,11 @@
       <c r="D95">
         <v>7</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>93</v>
       </c>
@@ -1989,8 +2250,11 @@
       <c r="D96">
         <v>7</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>94</v>
       </c>
@@ -2003,8 +2267,11 @@
       <c r="D97">
         <v>13</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>95</v>
       </c>
@@ -2017,8 +2284,11 @@
       <c r="D98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>96</v>
       </c>
@@ -2031,8 +2301,11 @@
       <c r="D99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>97</v>
       </c>
@@ -2045,8 +2318,11 @@
       <c r="D100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>98</v>
       </c>
@@ -2059,8 +2335,11 @@
       <c r="D101">
         <v>12</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>99</v>
       </c>
@@ -2073,8 +2352,11 @@
       <c r="D102">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>100</v>
       </c>
@@ -2087,8 +2369,11 @@
       <c r="D103">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>101</v>
       </c>
@@ -2101,8 +2386,11 @@
       <c r="D104">
         <v>7</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>102</v>
       </c>
@@ -2115,8 +2403,11 @@
       <c r="D105">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>103</v>
       </c>
@@ -2129,8 +2420,11 @@
       <c r="D106">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>104</v>
       </c>
@@ -2143,8 +2437,11 @@
       <c r="D107">
         <v>11</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>105</v>
       </c>
@@ -2157,8 +2454,11 @@
       <c r="D108">
         <v>3</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>106</v>
       </c>
@@ -2171,8 +2471,11 @@
       <c r="D109">
         <v>4</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>107</v>
       </c>
@@ -2185,8 +2488,11 @@
       <c r="D110">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>108</v>
       </c>
@@ -2199,8 +2505,11 @@
       <c r="D111">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>109</v>
       </c>
@@ -2213,8 +2522,11 @@
       <c r="D112">
         <v>11</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>110</v>
       </c>
@@ -2227,8 +2539,11 @@
       <c r="D113">
         <v>12</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>111</v>
       </c>
@@ -2241,8 +2556,11 @@
       <c r="D114">
         <v>3</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>112</v>
       </c>
@@ -2255,8 +2573,11 @@
       <c r="D115">
         <v>4</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>113</v>
       </c>
@@ -2269,8 +2590,11 @@
       <c r="D116">
         <v>3</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>114</v>
       </c>
@@ -2283,8 +2607,11 @@
       <c r="D117">
         <v>4</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>115</v>
       </c>
@@ -2297,8 +2624,11 @@
       <c r="D118">
         <v>12</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>116</v>
       </c>
@@ -2311,8 +2641,11 @@
       <c r="D119">
         <v>10</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>117</v>
       </c>
@@ -2325,8 +2658,11 @@
       <c r="D120">
         <v>11</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>118</v>
       </c>
@@ -2339,8 +2675,11 @@
       <c r="D121">
         <v>12</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>119</v>
       </c>
@@ -2353,8 +2692,11 @@
       <c r="D122">
         <v>13</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>120</v>
       </c>
@@ -2367,8 +2709,11 @@
       <c r="D123">
         <v>11</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>121</v>
       </c>
@@ -2381,8 +2726,11 @@
       <c r="D124">
         <v>12</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>122</v>
       </c>
@@ -2395,8 +2743,11 @@
       <c r="D125">
         <v>12</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>123</v>
       </c>
@@ -2409,8 +2760,11 @@
       <c r="D126">
         <v>1</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>124</v>
       </c>
@@ -2423,8 +2777,11 @@
       <c r="D127">
         <v>13</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>125</v>
       </c>
@@ -2437,8 +2794,11 @@
       <c r="D128">
         <v>12</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>126</v>
       </c>
@@ -2451,8 +2811,11 @@
       <c r="D129">
         <v>13</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>127</v>
       </c>
@@ -2465,8 +2828,11 @@
       <c r="D130">
         <v>11</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>128</v>
       </c>
@@ -2479,8 +2845,11 @@
       <c r="D131">
         <v>13</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>129</v>
       </c>
@@ -2493,8 +2862,11 @@
       <c r="D132">
         <v>12</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>130</v>
       </c>
@@ -2507,8 +2879,11 @@
       <c r="D133">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>131</v>
       </c>
@@ -2521,8 +2896,11 @@
       <c r="D134">
         <v>4</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>132</v>
       </c>
@@ -2535,8 +2913,11 @@
       <c r="D135">
         <v>10</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>133</v>
       </c>
@@ -2550,7 +2931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>134</v>
       </c>
@@ -2564,7 +2945,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>135</v>
       </c>
@@ -2578,7 +2959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>136</v>
       </c>
@@ -2592,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>137</v>
       </c>
@@ -2606,7 +2987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>138</v>
       </c>
@@ -2620,7 +3001,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>139</v>
       </c>
@@ -2634,7 +3015,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>140</v>
       </c>
@@ -2648,7 +3029,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>141</v>
       </c>
@@ -2943,7 +3324,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>